<commit_message>
Create and Delete Route Added
</commit_message>
<xml_diff>
--- a/DataLA.xlsx
+++ b/DataLA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21860" yWindow="4140" windowWidth="20240" windowHeight="17960" tabRatio="500"/>
+    <workbookView xWindow="25300" yWindow="12840" windowWidth="12780" windowHeight="9440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Login Info" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>URL:</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Adjustresolution:</t>
+  </si>
+  <si>
+    <t>Jenkins</t>
   </si>
 </sst>
 </file>
@@ -471,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,7 +487,7 @@
     <col min="4" max="4" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -497,8 +500,11 @@
       <c r="D1" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -511,32 +517,35 @@
       <c r="D2" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>

</xml_diff>

<commit_message>
Update Test Suite Script
</commit_message>
<xml_diff>
--- a/DataLA.xlsx
+++ b/DataLA.xlsx
@@ -477,7 +477,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -515,7 +515,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Update with new legend test
</commit_message>
<xml_diff>
--- a/DataLA.xlsx
+++ b/DataLA.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25300" yWindow="12840" windowWidth="12780" windowHeight="9440" tabRatio="500"/>
+    <workbookView xWindow="12060" yWindow="12400" windowWidth="18840" windowHeight="10140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Login Info" sheetId="1" r:id="rId1"/>
     <sheet name="VerifyMapLayers" sheetId="2" r:id="rId2"/>
+    <sheet name="VerifyLegend" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>URL:</t>
   </si>
@@ -145,6 +146,39 @@
   </si>
   <si>
     <t>Jenkins</t>
+  </si>
+  <si>
+    <t>Closure</t>
+  </si>
+  <si>
+    <t>Restriction</t>
+  </si>
+  <si>
+    <t>Crash</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>Coming Soon</t>
+  </si>
+  <si>
+    <t>Legend Icons:</t>
+  </si>
+  <si>
+    <t>Alts:</t>
+  </si>
+  <si>
+    <t>Img srcs:</t>
+  </si>
+  <si>
+    <t>Closure icon</t>
+  </si>
+  <si>
+    <t>Restriction icon</t>
   </si>
 </sst>
 </file>
@@ -477,7 +511,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -742,4 +776,97 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update with double wait functions
</commit_message>
<xml_diff>
--- a/DataLA.xlsx
+++ b/DataLA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15400" yWindow="5480" windowWidth="15260" windowHeight="11300" tabRatio="500"/>
+    <workbookView xWindow="-15820" yWindow="960" windowWidth="15260" windowHeight="11300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Login Info" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update LA Legend Test
</commit_message>
<xml_diff>
--- a/DataLA.xlsx
+++ b/DataLA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-16660" yWindow="600" windowWidth="16500" windowHeight="15060" tabRatio="500"/>
+    <workbookView xWindow="-17020" yWindow="1400" windowWidth="16500" windowHeight="11360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Login Info" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,7 +549,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>

</xml_diff>